<commit_message>
New_DNN 수정(accuracy 같은 문제)
</commit_message>
<xml_diff>
--- a/DNN/PFMatrix.xlsx
+++ b/DNN/PFMatrix.xlsx
@@ -484,46 +484,46 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>33.33333333333333</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>33.33333333333333</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>33.33333333333333</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>33.33333333333333</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>33.33333333333333</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>33.33333333333333</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>33.33333333333333</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>33.33333333333333</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>33.33333333333333</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>33.33333333333333</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>33.33333333333333</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="N2" t="n">
-        <v>0</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>0.3333333333333334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>